<commit_message>
- created Analysis file - edited data file
</commit_message>
<xml_diff>
--- a/data/versaceSales.xlsx
+++ b/data/versaceSales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hortenciahernandez/Desktop/versace_sales/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3F4CD30-0C3E-6348-A297-D19E9EB62996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{0FD91D9C-330C-4B47-86C1-7C9DFB4EBBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3680" yWindow="1060" windowWidth="23140" windowHeight="16940" activeTab="2" xr2:uid="{7C4450A4-67DB-8048-8026-FA224A955C7D}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="49">
   <si>
     <t>Total</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Q3</t>
+  </si>
+  <si>
+    <t>End Date</t>
   </si>
 </sst>
 </file>
@@ -2189,7 +2192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A89EC793-A620-004B-87AE-5F2798DD3CA9}">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D76" sqref="A1:D76"/>
     </sheetView>
   </sheetViews>
@@ -3270,10 +3273,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62F2D8C-70C5-F041-973D-1B4919CF47F3}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3282,7 +3285,7 @@
     <col min="2" max="2" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -3298,8 +3301,11 @@
       <c r="E1" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -3315,8 +3321,11 @@
       <c r="E2" s="1">
         <v>43640</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="1">
+        <v>43687</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -3333,7 +3342,7 @@
         <v>45017</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -3350,7 +3359,7 @@
         <v>45017</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3367,7 +3376,7 @@
         <v>45127</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -3384,7 +3393,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -3401,7 +3410,7 @@
         <v>45320</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -3418,7 +3427,7 @@
         <v>45330</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -3435,7 +3444,7 @@
         <v>45352</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -3452,7 +3461,7 @@
         <v>45364</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -3469,7 +3478,7 @@
         <v>45433</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -3486,7 +3495,7 @@
         <v>45490</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -3503,7 +3512,7 @@
         <v>45627</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>

</xml_diff>